<commit_message>
Updated variables and Excel data
</commit_message>
<xml_diff>
--- a/RoSATron/ExcelData/RoSATarget.xlsx
+++ b/RoSATron/ExcelData/RoSATarget.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Programming\Revature\Revature UIPath Batch\Embrey_J_Krasner_A-P0\RoSATron\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E64D254-280B-4D2E-A9BE-C07F19215495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD63799-3EAE-48CC-AAA1-D05C33E6596F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5614C46B-DE10-4F57-A84F-ACD1034DA0F1}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5614C46B-DE10-4F57-A84F-ACD1034DA0F1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Products" sheetId="1" r:id="rId1"/>
+    <sheet name="Vendors" sheetId="1" r:id="rId1"/>
     <sheet name="Clients" sheetId="2" r:id="rId2"/>
     <sheet name="Expenses" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="Cost">Products!$B:$B</definedName>
-    <definedName name="Produce">Products!$A:$A</definedName>
+    <definedName name="Cost">Vendors!$B:$B</definedName>
+    <definedName name="Produce">Vendors!$A:$A</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,14 +40,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Eggs</t>
   </si>
   <si>
-    <t>1 lb. Sliced Bacon</t>
-  </si>
-  <si>
     <t>Cinnamon Toast Crunch</t>
   </si>
   <si>
@@ -103,6 +100,42 @@
   </si>
   <si>
     <t>Semaj</t>
+  </si>
+  <si>
+    <t>JP</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Early Bird Produce</t>
+  </si>
+  <si>
+    <t>The Entertainer</t>
+  </si>
+  <si>
+    <t>Fight Club</t>
+  </si>
+  <si>
+    <t>Dark Side of the Moon Vinyl</t>
+  </si>
+  <si>
+    <t>Zelda BOTW</t>
+  </si>
+  <si>
+    <t>Technotrocity</t>
+  </si>
+  <si>
+    <t>Samsung S9000</t>
+  </si>
+  <si>
+    <t>Tile Mate</t>
+  </si>
+  <si>
+    <t>Oculus Quest 2</t>
+  </si>
+  <si>
+    <t>Sliced Bacon</t>
   </si>
 </sst>
 </file>
@@ -505,60 +538,174 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5DC2EA3-C148-42E5-9646-070198748FCC}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G1" s="3"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+    </row>
+    <row r="2" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
+      <c r="C2" s="2">
         <v>1.6</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>120</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="G2" s="1"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="2">
+        <v>5.83</v>
+      </c>
+      <c r="D3">
+        <v>100</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
-        <v>5.83</v>
-      </c>
-      <c r="C3">
+      <c r="C4" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="D4">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="C4">
-        <v>50</v>
-      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="2">
+        <v>40</v>
+      </c>
+      <c r="D7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="2">
+        <v>25</v>
+      </c>
+      <c r="D8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="2">
+        <v>900</v>
+      </c>
+      <c r="D10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
+      <c r="B11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="2">
+        <v>25</v>
+      </c>
+      <c r="D11">
+        <v>100</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="2">
+        <v>300</v>
+      </c>
+      <c r="D12">
+        <v>100</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -568,10 +715,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0026A6E-D28A-4737-9C9E-9F29273C5BC1}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,13 +729,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -596,7 +743,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -604,6 +751,14 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -626,10 +781,10 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -637,10 +792,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -648,10 +803,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -659,10 +814,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -670,10 +825,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pretty much fully laid out Welcome screen. Got all inventory to decrement
</commit_message>
<xml_diff>
--- a/RoSATron/ExcelData/RoSATarget.xlsx
+++ b/RoSATron/ExcelData/RoSATarget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Programming\Revature\Revature UIPath Batch\Embrey_J_Krasner_A-P0\RoSATron\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD63799-3EAE-48CC-AAA1-D05C33E6596F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62D6869-CDB1-4CA0-8EDB-1BA0B97F5B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5614C46B-DE10-4F57-A84F-ACD1034DA0F1}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>Eggs</t>
   </si>
@@ -57,85 +57,124 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>Jason</t>
-  </si>
-  <si>
-    <t>Brody</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>Mark</t>
-  </si>
-  <si>
-    <t>Hopper</t>
-  </si>
-  <si>
-    <t>Janis</t>
-  </si>
-  <si>
-    <t>Joplin</t>
-  </si>
-  <si>
-    <t>Jimi</t>
-  </si>
-  <si>
-    <t>Hendrix</t>
-  </si>
-  <si>
     <t>ClientName</t>
   </si>
   <si>
+    <t>ClientID</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Early Bird Produce</t>
+  </si>
+  <si>
+    <t>The Entertainer</t>
+  </si>
+  <si>
+    <t>Fight Club</t>
+  </si>
+  <si>
+    <t>Dark Side of the Moon Vinyl</t>
+  </si>
+  <si>
+    <t>Zelda BOTW</t>
+  </si>
+  <si>
+    <t>Technotrocity</t>
+  </si>
+  <si>
+    <t>Samsung S9000</t>
+  </si>
+  <si>
+    <t>Tile Mate</t>
+  </si>
+  <si>
+    <t>Oculus Quest 2</t>
+  </si>
+  <si>
+    <t>Sliced Bacon</t>
+  </si>
+  <si>
     <t>Column1</t>
   </si>
   <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>ProductQuantity</t>
+  </si>
+  <si>
+    <t>Rosa</t>
+  </si>
+  <si>
+    <t>Cheddar</t>
+  </si>
+  <si>
+    <t>GZA</t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>qwerty</t>
+  </si>
+  <si>
+    <t>zxcv</t>
+  </si>
+  <si>
+    <t>wert</t>
+  </si>
+  <si>
+    <t>ty</t>
+  </si>
+  <si>
+    <t>fgh</t>
+  </si>
+  <si>
+    <t>Guy</t>
+  </si>
+  <si>
+    <t>Scully</t>
+  </si>
+  <si>
+    <t>JP</t>
+  </si>
+  <si>
     <t>James</t>
   </si>
   <si>
-    <t>ClientID</t>
-  </si>
-  <si>
-    <t>Semaj</t>
-  </si>
-  <si>
-    <t>JP</t>
-  </si>
-  <si>
-    <t>Vendor</t>
-  </si>
-  <si>
-    <t>Early Bird Produce</t>
-  </si>
-  <si>
-    <t>The Entertainer</t>
-  </si>
-  <si>
-    <t>Fight Club</t>
-  </si>
-  <si>
-    <t>Dark Side of the Moon Vinyl</t>
-  </si>
-  <si>
-    <t>Zelda BOTW</t>
-  </si>
-  <si>
-    <t>Technotrocity</t>
-  </si>
-  <si>
-    <t>Samsung S9000</t>
-  </si>
-  <si>
-    <t>Tile Mate</t>
-  </si>
-  <si>
-    <t>Oculus Quest 2</t>
-  </si>
-  <si>
-    <t>Sliced Bacon</t>
+    <t>GUy</t>
+  </si>
+  <si>
+    <t>Garrison</t>
+  </si>
+  <si>
+    <t>Gha</t>
+  </si>
+  <si>
+    <t>Fuh</t>
+  </si>
+  <si>
+    <t>Jameson</t>
+  </si>
+  <si>
+    <t>Gus</t>
+  </si>
+  <si>
+    <t>Hue Jass</t>
+  </si>
+  <si>
+    <t>Faygo</t>
+  </si>
+  <si>
+    <t>Roger</t>
+  </si>
+  <si>
+    <t>Qubert</t>
   </si>
 </sst>
 </file>
@@ -541,7 +580,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,7 +591,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>3</v>
@@ -569,7 +608,7 @@
     </row>
     <row r="2" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -578,7 +617,7 @@
         <v>1.6</v>
       </c>
       <c r="D2">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="2"/>
@@ -586,7 +625,7 @@
     <row r="3" spans="1:9" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2">
         <v>5.83</v>
@@ -611,13 +650,17 @@
       <c r="G4" s="1"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>100</v>
+      </c>
+    </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2">
         <v>7</v>
@@ -629,7 +672,7 @@
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C7" s="2">
         <v>40</v>
@@ -641,7 +684,7 @@
     <row r="8" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C8" s="2">
         <v>25</v>
@@ -654,13 +697,16 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
+      <c r="D9">
+        <v>100</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="C10" s="2">
         <v>900</v>
@@ -672,7 +718,7 @@
     <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C11" s="2">
         <v>25</v>
@@ -686,7 +732,7 @@
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="C12" s="2">
         <v>300</v>
@@ -715,10 +761,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0026A6E-D28A-4737-9C9E-9F29273C5BC1}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,13 +775,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -743,7 +789,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -751,7 +797,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -759,7 +805,199 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -770,68 +1008,36 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C174ED6F-399B-4FEA-94EA-7AFBD1091A71}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
+      <c r="C1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
On top of being able to add clients to existing client list, RoSA also takes email and client orders from vendors and adds them to expense report. Also detects items not found or out of stock
</commit_message>
<xml_diff>
--- a/RoSATron/ExcelData/RoSATarget.xlsx
+++ b/RoSATron/ExcelData/RoSATarget.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Programming\Revature\Revature UIPath Batch\Embrey_J_Krasner_A-P0\RoSATron\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62D6869-CDB1-4CA0-8EDB-1BA0B97F5B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1938A23D-C059-477F-B9EA-577F0DD13947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5614C46B-DE10-4F57-A84F-ACD1034DA0F1}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5614C46B-DE10-4F57-A84F-ACD1034DA0F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Vendors" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
   <si>
     <t>Eggs</t>
   </si>
@@ -60,9 +60,6 @@
     <t>ClientName</t>
   </si>
   <si>
-    <t>ClientID</t>
-  </si>
-  <si>
     <t>Vendor</t>
   </si>
   <si>
@@ -105,76 +102,64 @@
     <t>ProductQuantity</t>
   </si>
   <si>
-    <t>Rosa</t>
-  </si>
-  <si>
-    <t>Cheddar</t>
-  </si>
-  <si>
-    <t>GZA</t>
-  </si>
-  <si>
-    <t>asdf</t>
-  </si>
-  <si>
-    <t>Doe</t>
-  </si>
-  <si>
-    <t>qwerty</t>
-  </si>
-  <si>
-    <t>zxcv</t>
-  </si>
-  <si>
-    <t>wert</t>
-  </si>
-  <si>
-    <t>ty</t>
-  </si>
-  <si>
-    <t>fgh</t>
-  </si>
-  <si>
-    <t>Guy</t>
-  </si>
-  <si>
-    <t>Scully</t>
+    <t>TotalCost</t>
+  </si>
+  <si>
+    <t>ClientEmail</t>
   </si>
   <si>
     <t>JP</t>
   </si>
   <si>
+    <t>jpat.embrey@gmail.com</t>
+  </si>
+  <si>
     <t>James</t>
   </si>
   <si>
-    <t>GUy</t>
-  </si>
-  <si>
-    <t>Garrison</t>
-  </si>
-  <si>
-    <t>Gha</t>
-  </si>
-  <si>
-    <t>Fuh</t>
+    <t>james.embrey@revature.net</t>
+  </si>
+  <si>
+    <t>Semaj</t>
+  </si>
+  <si>
+    <t>semaj.james@gmail.com</t>
   </si>
   <si>
     <t>Jameson</t>
   </si>
   <si>
-    <t>Gus</t>
-  </si>
-  <si>
-    <t>Hue Jass</t>
-  </si>
-  <si>
-    <t>Faygo</t>
-  </si>
-  <si>
-    <t>Roger</t>
-  </si>
-  <si>
-    <t>Qubert</t>
+    <t>jameson.whiskey@gmail.com</t>
+  </si>
+  <si>
+    <t>Jesam</t>
+  </si>
+  <si>
+    <t>jesam.yember@gmail.com</t>
+  </si>
+  <si>
+    <t>Falcon</t>
+  </si>
+  <si>
+    <t>captain.falcon@gmail.com</t>
+  </si>
+  <si>
+    <t>Jamie</t>
+  </si>
+  <si>
+    <t>jamie.embrey@gmail.com</t>
+  </si>
+  <si>
+    <t>Ghastly</t>
+  </si>
+  <si>
+    <t>ghastly.pokemon@gmail.com</t>
+  </si>
+  <si>
+    <t>VRJames</t>
+  </si>
+  <si>
+    <t>vr.james@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -579,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5DC2EA3-C148-42E5-9646-070198748FCC}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,7 +576,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>3</v>
@@ -608,7 +593,7 @@
     </row>
     <row r="2" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -617,7 +602,7 @@
         <v>1.6</v>
       </c>
       <c r="D2">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="2"/>
@@ -625,13 +610,13 @@
     <row r="3" spans="1:9" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2">
         <v>5.83</v>
       </c>
       <c r="D3">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="2"/>
@@ -645,86 +630,79 @@
         <v>2.5</v>
       </c>
       <c r="D4">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D5">
-        <v>100</v>
-      </c>
-    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="C6" s="2">
         <v>7</v>
       </c>
       <c r="D6">
-        <v>100</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="2">
         <v>40</v>
       </c>
       <c r="D7">
-        <v>100</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="2">
         <v>25</v>
       </c>
       <c r="D8">
-        <v>100</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
-      <c r="D9">
-        <v>100</v>
-      </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="C10" s="2">
         <v>900</v>
       </c>
       <c r="D10">
-        <v>100</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="2">
         <v>25</v>
       </c>
       <c r="D11">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="2"/>
@@ -732,13 +710,13 @@
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="2">
         <v>300</v>
       </c>
       <c r="D12">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="2"/>
@@ -761,243 +739,99 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0026A6E-D28A-4737-9C9E-9F29273C5BC1}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B12" sqref="A2:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
+      <c r="A3" t="s">
+        <v>24</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
+      <c r="A4" t="s">
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
+      <c r="A5" t="s">
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1</v>
+      <c r="A6" t="s">
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1</v>
+      <c r="A7" t="s">
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1</v>
+      <c r="A8" t="s">
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1</v>
+      <c r="A9" t="s">
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1</v>
+      <c r="A10" t="s">
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>1</v>
-      </c>
-      <c r="B22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>1</v>
-      </c>
-      <c r="B24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>1</v>
-      </c>
-      <c r="B25" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>1</v>
-      </c>
-      <c r="B26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>1</v>
-      </c>
-      <c r="B27" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1008,32 +842,158 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C174ED6F-399B-4FEA-94EA-7AFBD1091A71}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D12" sqref="A2:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>69.959999999999994</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>10800</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <v>3600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RoSA can now add vendors along with 3 products, including each products cost and quantity.
</commit_message>
<xml_diff>
--- a/RoSATron/ExcelData/RoSATarget.xlsx
+++ b/RoSATron/ExcelData/RoSATarget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Programming\Revature\Revature UIPath Batch\Embrey_J_Krasner_A-P0\RoSATron\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1938A23D-C059-477F-B9EA-577F0DD13947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5045C18-7F5B-481B-B8DF-9A464DC76CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5614C46B-DE10-4F57-A84F-ACD1034DA0F1}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5614C46B-DE10-4F57-A84F-ACD1034DA0F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Vendors" sheetId="1" r:id="rId1"/>
@@ -63,103 +63,103 @@
     <t>Vendor</t>
   </si>
   <si>
+    <t>The Entertainer</t>
+  </si>
+  <si>
+    <t>Fight Club</t>
+  </si>
+  <si>
+    <t>Dark Side of the Moon Vinyl</t>
+  </si>
+  <si>
+    <t>Zelda BOTW</t>
+  </si>
+  <si>
+    <t>Technotrocity</t>
+  </si>
+  <si>
+    <t>Samsung S9000</t>
+  </si>
+  <si>
+    <t>Tile Mate</t>
+  </si>
+  <si>
+    <t>Oculus Quest 2</t>
+  </si>
+  <si>
+    <t>Sliced Bacon</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>ProductQuantity</t>
+  </si>
+  <si>
+    <t>TotalCost</t>
+  </si>
+  <si>
+    <t>ClientEmail</t>
+  </si>
+  <si>
+    <t>jpat.embrey@gmail.com</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>james.embrey@revature.net</t>
+  </si>
+  <si>
     <t>Early Bird Produce</t>
   </si>
   <si>
-    <t>The Entertainer</t>
-  </si>
-  <si>
-    <t>Fight Club</t>
-  </si>
-  <si>
-    <t>Dark Side of the Moon Vinyl</t>
-  </si>
-  <si>
-    <t>Zelda BOTW</t>
-  </si>
-  <si>
-    <t>Technotrocity</t>
-  </si>
-  <si>
-    <t>Samsung S9000</t>
-  </si>
-  <si>
-    <t>Tile Mate</t>
-  </si>
-  <si>
-    <t>Oculus Quest 2</t>
-  </si>
-  <si>
-    <t>Sliced Bacon</t>
-  </si>
-  <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t>ProductName</t>
-  </si>
-  <si>
-    <t>ProductQuantity</t>
-  </si>
-  <si>
-    <t>TotalCost</t>
-  </si>
-  <si>
-    <t>ClientEmail</t>
-  </si>
-  <si>
-    <t>JP</t>
-  </si>
-  <si>
-    <t>jpat.embrey@gmail.com</t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
-    <t>james.embrey@revature.net</t>
-  </si>
-  <si>
-    <t>Semaj</t>
-  </si>
-  <si>
-    <t>semaj.james@gmail.com</t>
-  </si>
-  <si>
-    <t>Jameson</t>
-  </si>
-  <si>
-    <t>jameson.whiskey@gmail.com</t>
-  </si>
-  <si>
-    <t>Jesam</t>
-  </si>
-  <si>
-    <t>jesam.yember@gmail.com</t>
-  </si>
-  <si>
-    <t>Falcon</t>
-  </si>
-  <si>
-    <t>captain.falcon@gmail.com</t>
-  </si>
-  <si>
-    <t>Jamie</t>
-  </si>
-  <si>
-    <t>jamie.embrey@gmail.com</t>
-  </si>
-  <si>
-    <t>Ghastly</t>
-  </si>
-  <si>
-    <t>ghastly.pokemon@gmail.com</t>
-  </si>
-  <si>
-    <t>VRJames</t>
-  </si>
-  <si>
-    <t>vr.james@gmail.com</t>
+    <t>James Embrey</t>
+  </si>
+  <si>
+    <t>fuzzynutz</t>
+  </si>
+  <si>
+    <t>hot.fuzz@dmail.com</t>
+  </si>
+  <si>
+    <t>Psyntst</t>
+  </si>
+  <si>
+    <t>psyntfcwhun@gmail.com</t>
+  </si>
+  <si>
+    <t>Rosa</t>
+  </si>
+  <si>
+    <t>rosa@gmail.com</t>
+  </si>
+  <si>
+    <t>Jake</t>
+  </si>
+  <si>
+    <t>jake.99@gmail.com</t>
+  </si>
+  <si>
+    <t>Amy Santiago</t>
+  </si>
+  <si>
+    <t>SAmy.99@bmail.com</t>
+  </si>
+  <si>
+    <t>Terry Crews</t>
+  </si>
+  <si>
+    <t>terryterry@gmail.com</t>
+  </si>
+  <si>
+    <t>Holt</t>
+  </si>
+  <si>
+    <t>rayholt@b99mail.com</t>
   </si>
 </sst>
 </file>
@@ -562,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5DC2EA3-C148-42E5-9646-070198748FCC}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D25" sqref="A17:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,7 +593,7 @@
     </row>
     <row r="2" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -602,7 +602,7 @@
         <v>1.6</v>
       </c>
       <c r="D2">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="2"/>
@@ -610,13 +610,13 @@
     <row r="3" spans="1:9" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2">
         <v>5.83</v>
       </c>
       <c r="D3">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="2"/>
@@ -630,106 +630,109 @@
         <v>2.5</v>
       </c>
       <c r="D4">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>88</v>
+      </c>
+    </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="D6">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2">
+        <v>25</v>
+      </c>
+      <c r="D7">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="2">
-        <v>40</v>
-      </c>
-      <c r="D7">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C8" s="2">
+        <v>900</v>
+      </c>
+      <c r="D8">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="2">
         <v>25</v>
       </c>
-      <c r="D8">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="2"/>
+      <c r="D9">
+        <v>88</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10" s="2">
-        <v>900</v>
+        <v>300</v>
       </c>
       <c r="D10">
-        <v>83</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="2">
-        <v>25</v>
-      </c>
-      <c r="D11">
-        <v>78</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="2"/>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="2">
-        <v>300</v>
-      </c>
-      <c r="D12">
-        <v>83</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C15" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -742,12 +745,12 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B12" sqref="A2:B12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
   </cols>
   <sheetData>
@@ -756,42 +759,42 @@
         <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -844,13 +847,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C174ED6F-399B-4FEA-94EA-7AFBD1091A71}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D12" sqref="A2:D12"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" customWidth="1"/>
@@ -861,18 +864,18 @@
         <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -886,10 +889,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3">
         <v>12</v>
@@ -900,7 +903,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -914,10 +917,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>12</v>
@@ -931,7 +934,7 @@
         <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <v>12</v>
@@ -945,7 +948,7 @@
         <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>12</v>
@@ -959,7 +962,7 @@
         <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8">
         <v>12</v>
@@ -973,7 +976,7 @@
         <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>12</v>
@@ -987,7 +990,7 @@
         <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <v>12</v>

</xml_diff>

<commit_message>
RoSA now calculates discounts for products
</commit_message>
<xml_diff>
--- a/RoSATron/ExcelData/RoSATarget.xlsx
+++ b/RoSATron/ExcelData/RoSATarget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Programming\Revature\Revature UIPath Batch\Embrey_J_Krasner_A-P0\RoSATron\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5045C18-7F5B-481B-B8DF-9A464DC76CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18648398-E842-4F38-A7EF-A094B75AAA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5614C46B-DE10-4F57-A84F-ACD1034DA0F1}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5614C46B-DE10-4F57-A84F-ACD1034DA0F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Vendors" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
   <si>
     <t>Eggs</t>
   </si>
@@ -72,24 +72,15 @@
     <t>Dark Side of the Moon Vinyl</t>
   </si>
   <si>
-    <t>Zelda BOTW</t>
-  </si>
-  <si>
     <t>Technotrocity</t>
   </si>
   <si>
     <t>Samsung S9000</t>
   </si>
   <si>
-    <t>Tile Mate</t>
-  </si>
-  <si>
     <t>Oculus Quest 2</t>
   </si>
   <si>
-    <t>Sliced Bacon</t>
-  </si>
-  <si>
     <t>Column1</t>
   </si>
   <si>
@@ -160,6 +151,87 @@
   </si>
   <si>
     <t>rayholt@b99mail.com</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tile Mate </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(10% Discount)</t>
+    </r>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>john@gmail.com</t>
+  </si>
+  <si>
+    <t>rosa@99.com</t>
+  </si>
+  <si>
+    <t>Faye</t>
+  </si>
+  <si>
+    <t>faye.valentine@gmail.com</t>
+  </si>
+  <si>
+    <t>james.embrey@gmail.com</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Zelda BOTW </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(5% Discount)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sliced Bacon </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(2% Discount)</t>
+    </r>
+  </si>
+  <si>
+    <t>James Bond</t>
+  </si>
+  <si>
+    <t>james.bond@mi6.com</t>
+  </si>
+  <si>
+    <t>James Patrick Embrey</t>
+  </si>
+  <si>
+    <t>james.patrick.embrey@embrey.net</t>
+  </si>
+  <si>
+    <t>JPE</t>
+  </si>
+  <si>
+    <t>jpe@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -564,14 +636,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5DC2EA3-C148-42E5-9646-070198748FCC}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D25" sqref="A17:D25"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -593,16 +665,16 @@
     </row>
     <row r="2" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>1.6</v>
       </c>
       <c r="D2">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="2"/>
@@ -610,9 +682,9 @@
     <row r="3" spans="1:9" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="2">
+        <v>45</v>
+      </c>
+      <c r="C3">
         <v>5.83</v>
       </c>
       <c r="D3">
@@ -626,11 +698,11 @@
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>2.5</v>
       </c>
       <c r="D4">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="2"/>
@@ -642,23 +714,23 @@
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>7</v>
       </c>
       <c r="D5">
-        <v>88</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="2">
-        <v>40</v>
+        <v>44</v>
+      </c>
+      <c r="C6">
+        <v>39.99</v>
       </c>
       <c r="D6">
-        <v>88</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -666,37 +738,37 @@
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2">
-        <v>25</v>
+      <c r="C7">
+        <v>24.99</v>
       </c>
       <c r="D7">
-        <v>88</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="2">
-        <v>900</v>
+      <c r="C8">
+        <v>899.99</v>
       </c>
       <c r="D8">
-        <v>88</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="2">
-        <v>25</v>
+        <v>37</v>
+      </c>
+      <c r="C9" s="1">
+        <v>24.99</v>
       </c>
       <c r="D9">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="2"/>
@@ -704,13 +776,13 @@
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="2">
+        <v>12</v>
+      </c>
+      <c r="C10" s="1">
         <v>300</v>
       </c>
       <c r="D10">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="2"/>
@@ -742,7 +814,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0026A6E-D28A-4737-9C9E-9F29273C5BC1}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
@@ -759,82 +831,146 @@
         <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>38</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -845,16 +981,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C174ED6F-399B-4FEA-94EA-7AFBD1091A71}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D17" sqref="A2:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" customWidth="1"/>
   </cols>
@@ -864,139 +1000,13 @@
         <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>12</v>
-      </c>
-      <c r="D2">
-        <v>19.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3">
-        <v>12</v>
-      </c>
-      <c r="D3">
-        <v>69.959999999999994</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>12</v>
-      </c>
-      <c r="D4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>12</v>
-      </c>
-      <c r="D5">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6">
-        <v>12</v>
-      </c>
-      <c r="D6">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7">
-        <v>12</v>
-      </c>
-      <c r="D7">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8">
-        <v>12</v>
-      </c>
-      <c r="D8">
-        <v>10800</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9">
-        <v>12</v>
-      </c>
-      <c r="D9">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10">
-        <v>12</v>
-      </c>
-      <c r="D10">
-        <v>3600</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed an issue with finding products. RoSA can now detect when a product is not found.
</commit_message>
<xml_diff>
--- a/RoSATron/ExcelData/RoSATarget.xlsx
+++ b/RoSATron/ExcelData/RoSATarget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Programming\Revature\Revature UIPath Batch\Embrey_J_Krasner_A-P0\RoSATron\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18648398-E842-4F38-A7EF-A094B75AAA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AB1B8C-1123-4C88-A799-9A47B175D969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5614C46B-DE10-4F57-A84F-ACD1034DA0F1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5614C46B-DE10-4F57-A84F-ACD1034DA0F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Vendors" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="64">
   <si>
     <t>Eggs</t>
   </si>
@@ -232,6 +232,42 @@
   </si>
   <si>
     <t>jpe@gmail.com</t>
+  </si>
+  <si>
+    <t>Ai Krasner</t>
+  </si>
+  <si>
+    <t>ai.krasner@gmail.com</t>
+  </si>
+  <si>
+    <t>Zelda BOTW (5% Discount)</t>
+  </si>
+  <si>
+    <t>jake.peralta@gmail.com</t>
+  </si>
+  <si>
+    <t>Soda City</t>
+  </si>
+  <si>
+    <t>Surge</t>
+  </si>
+  <si>
+    <t>Mountain Dew</t>
+  </si>
+  <si>
+    <t>Pepsi</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>Bicycle</t>
+  </si>
+  <si>
+    <t>Washing Machine</t>
+  </si>
+  <si>
+    <t>Basket</t>
   </si>
 </sst>
 </file>
@@ -634,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5DC2EA3-C148-42E5-9646-070198748FCC}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,7 +724,7 @@
         <v>5.83</v>
       </c>
       <c r="D3">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="2"/>
@@ -730,7 +766,7 @@
         <v>39.99</v>
       </c>
       <c r="D6">
-        <v>76</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -805,6 +841,78 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16">
+        <v>5.99</v>
+      </c>
+      <c r="D16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17">
+        <v>5.99</v>
+      </c>
+      <c r="D17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18">
+        <v>7.99</v>
+      </c>
+      <c r="D18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19">
+        <v>99.99</v>
+      </c>
+      <c r="D19">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20">
+        <v>149.99</v>
+      </c>
+      <c r="D20">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21">
+        <v>3.99</v>
+      </c>
+      <c r="D21">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -814,10 +922,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0026A6E-D28A-4737-9C9E-9F29273C5BC1}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B18" sqref="A2:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,6 +1081,30 @@
         <v>51</v>
       </c>
     </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -981,9 +1113,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C174ED6F-399B-4FEA-94EA-7AFBD1091A71}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D17" sqref="A2:D17"/>
     </sheetView>
   </sheetViews>
@@ -1009,6 +1141,34 @@
         <v>16</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>75.980999999999995</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Added multiple item purchases and made some various interface adjustments
</commit_message>
<xml_diff>
--- a/RoSATron/ExcelData/RoSATarget.xlsx
+++ b/RoSATron/ExcelData/RoSATarget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Programming\Revature\Revature UIPath Batch\Embrey_J_Krasner_A-P0\RoSATron\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45AB452E-B458-40CF-89D9-5704D2169EE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E12B2CE-4514-4645-BA08-91A5F70E52E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5614C46B-DE10-4F57-A84F-ACD1034DA0F1}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5614C46B-DE10-4F57-A84F-ACD1034DA0F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Vendors" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Eggs</t>
   </si>
@@ -141,52 +141,34 @@
     </r>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
     <t>JP</t>
   </si>
   <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Jameson</t>
+  </si>
+  <si>
+    <t>jameson.whiskey@gmail.com</t>
+  </si>
+  <si>
     <t>jpat.embrey@gmail.com</t>
   </si>
   <si>
-    <t>Guy</t>
-  </si>
-  <si>
-    <t>guy.sensei@gmail.com</t>
-  </si>
-  <si>
-    <t>Tess</t>
-  </si>
-  <si>
-    <t>tess.eract@gmail.com</t>
-  </si>
-  <si>
-    <t>Tile Mate (10% Discount)</t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
-    <t>james.embrey@revature.net</t>
-  </si>
-  <si>
-    <t>Ai</t>
-  </si>
-  <si>
-    <t>Ai.Krasner@revature.net</t>
-  </si>
-  <si>
-    <t>asdf</t>
-  </si>
-  <si>
-    <t>asdf@asdf.com</t>
-  </si>
-  <si>
-    <t>asdfasdf</t>
-  </si>
-  <si>
-    <t>Zelda BOTW (5% Discount)</t>
+    <t>jpatemb@gmail.com</t>
+  </si>
+  <si>
+    <t>pj</t>
+  </si>
+  <si>
+    <t>pjat</t>
+  </si>
+  <si>
+    <t>jp</t>
+  </si>
+  <si>
+    <t>jpat@emb</t>
   </si>
 </sst>
 </file>
@@ -261,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -274,7 +256,6 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5DC2EA3-C148-42E5-9646-070198748FCC}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D10"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,7 +610,7 @@
         <v>1.6</v>
       </c>
       <c r="D2">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="2"/>
@@ -657,7 +638,7 @@
         <v>2.5</v>
       </c>
       <c r="D4">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="2"/>
@@ -673,7 +654,7 @@
         <v>7</v>
       </c>
       <c r="D5">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -685,7 +666,7 @@
         <v>39.99</v>
       </c>
       <c r="D6">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -711,7 +692,7 @@
         <v>899.99</v>
       </c>
       <c r="D8">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -723,7 +704,7 @@
         <v>24.99</v>
       </c>
       <c r="D9">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="2"/>
@@ -769,99 +750,65 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0026A6E-D28A-4737-9C9E-9F29273C5BC1}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.28515625" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="5" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>26</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>29</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -872,10 +819,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C174ED6F-399B-4FEA-94EA-7AFBD1091A71}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,76 +847,6 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>12</v>
-      </c>
-      <c r="D2">
-        <v>19.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3">
-        <v>12</v>
-      </c>
-      <c r="D3">
-        <v>269.892</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>12</v>
-      </c>
-      <c r="D4">
-        <v>19.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>13.3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>75.980999999999995</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>